<commit_message>
chapter 6 expample 5
</commit_message>
<xml_diff>
--- a/src/Chapter-6/案例05 批量统计工作簿的最大、最小值/产品销售统计表.xlsx
+++ b/src/Chapter-6/案例05 批量统计工作簿的最大、最小值/产品销售统计表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\example\05\对一个工作簿中的全部工作表批量求和\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MGF\Documents\GitHub\TianXiaPy\PyExcel\src\Chapter-6\案例05 批量统计工作簿的最大、最小值\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F685AD9-51A8-482B-BCEE-5ED7839A6968}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AFF4EC-759E-4B35-9FE2-47756DD9CBCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8850" windowHeight="7620" tabRatio="955" activeTab="4" xr2:uid="{5116E507-4C83-441A-A83F-5DECC1ADA7D3}"/>
+    <workbookView xWindow="1020" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="955" activeTab="4" xr2:uid="{5116E507-4C83-441A-A83F-5DECC1ADA7D3}"/>
   </bookViews>
   <sheets>
     <sheet name="行李箱" sheetId="8" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="背包" sheetId="4" r:id="rId4"/>
     <sheet name="单肩包" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="32">
   <si>
     <t>产品名称</t>
   </si>
@@ -129,6 +129,13 @@
   <si>
     <t>销售利润</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大利润</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小利润</t>
   </si>
 </sst>
 </file>
@@ -190,7 +197,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -205,6 +212,12 @@
     </xf>
     <xf numFmtId="7" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,23 +533,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86E0DED-22AD-490C-AB8E-4EC951BD319E}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="13.44140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8" style="2"/>
+    <col min="1" max="1" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -561,8 +574,14 @@
       <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -587,8 +606,14 @@
       <c r="H2" s="4">
         <v>29700</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="4">
+        <v>57420</v>
+      </c>
+      <c r="J2" s="4">
+        <v>13860</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -614,7 +639,7 @@
         <v>56100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -640,7 +665,7 @@
         <v>36300</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -666,7 +691,7 @@
         <v>13860</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -692,7 +717,7 @@
         <v>52800</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -718,7 +743,7 @@
         <v>43560</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -744,7 +769,7 @@
         <v>15840</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -770,7 +795,7 @@
         <v>39600</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -796,7 +821,7 @@
         <v>39600</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -822,7 +847,7 @@
         <v>52800</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -848,7 +873,7 @@
         <v>46200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -883,25 +908,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08248075-C034-4AFB-B814-F8B910D4F45B}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="13.6640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8" style="1"/>
+    <col min="1" max="1" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -926,8 +951,14 @@
       <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -955,8 +986,14 @@
         <f>G2-F2</f>
         <v>48500</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="6">
+        <v>97000</v>
+      </c>
+      <c r="J2" s="6">
+        <v>34920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -985,7 +1022,7 @@
         <v>75660</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1014,7 +1051,7 @@
         <v>97000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1043,7 +1080,7 @@
         <v>34920</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1109,7 @@
         <v>43650</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1101,7 +1138,7 @@
         <v>67900</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1130,7 +1167,7 @@
         <v>46560</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1159,7 +1196,7 @@
         <v>54320</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1188,7 +1225,7 @@
         <v>58200</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1217,7 +1254,7 @@
         <v>46366</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1283,7 @@
         <v>77600</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1283,21 +1320,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD16AF4-FA4E-4AAE-B77A-CBE65ECFBC86}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" customWidth="1"/>
-    <col min="3" max="8" width="13.77734375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.109375" style="2"/>
+    <col min="1" max="1" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1322,8 +1363,14 @@
       <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1351,8 +1398,14 @@
         <f>G2-F2</f>
         <v>28860</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="4">
+        <v>99900</v>
+      </c>
+      <c r="J2" s="4">
+        <v>27750</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1381,7 +1434,7 @@
         <v>57720</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1410,7 +1463,7 @@
         <v>49950</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1439,7 +1492,7 @@
         <v>98790</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1468,7 +1521,7 @@
         <v>39960</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1497,7 +1550,7 @@
         <v>61050</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1526,7 +1579,7 @@
         <v>27750</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1555,7 +1608,7 @@
         <v>86580</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1584,7 +1637,7 @@
         <v>95460</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1613,7 +1666,7 @@
         <v>99900</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1642,7 +1695,7 @@
         <v>28638</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -1671,7 +1724,7 @@
         <v>66600</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F14" s="4"/>
     </row>
   </sheetData>
@@ -1682,21 +1735,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72D5B97-0FD7-47A4-B99D-C6BFD7277BDC}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10" style="2" customWidth="1"/>
-    <col min="3" max="8" width="13.33203125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="7.88671875" style="2"/>
+    <col min="1" max="1" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="7.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1721,8 +1777,14 @@
       <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1747,8 +1809,14 @@
       <c r="H2" s="4">
         <v>29400</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="4">
+        <v>39200</v>
+      </c>
+      <c r="J2" s="4">
+        <v>7350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1774,7 +1842,7 @@
         <v>11270</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1800,7 +1868,7 @@
         <v>12250</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1826,7 +1894,7 @@
         <v>33810</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1852,7 +1920,7 @@
         <v>26950</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1878,7 +1946,7 @@
         <v>27440</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1904,7 +1972,7 @@
         <v>7350</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1930,7 +1998,7 @@
         <v>19600</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1956,7 +2024,7 @@
         <v>17150</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1982,7 +2050,7 @@
         <v>36750</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -2008,7 +2076,7 @@
         <v>39200</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -2034,7 +2102,7 @@
         <v>30870</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="F14" s="4"/>
@@ -2049,21 +2117,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1842AE8A-FB92-4209-B731-09600CE6353E}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="2" customWidth="1"/>
-    <col min="3" max="8" width="12.88671875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="7.88671875" style="2"/>
+    <col min="1" max="1" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="7.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -2088,8 +2161,14 @@
       <c r="H1" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2117,8 +2196,14 @@
         <f>G2-F2</f>
         <v>41580</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="4">
+        <v>57420</v>
+      </c>
+      <c r="J2" s="4">
+        <v>9570</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -2147,7 +2232,7 @@
         <v>38280</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2176,7 +2261,7 @@
         <v>13200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -2205,7 +2290,7 @@
         <v>41580</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -2234,7 +2319,7 @@
         <v>39600</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -2263,7 +2348,7 @@
         <v>51480</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -2292,7 +2377,7 @@
         <v>13200</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -2321,7 +2406,7 @@
         <v>45540</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -2350,7 +2435,7 @@
         <v>33000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -2379,7 +2464,7 @@
         <v>57420</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -2408,7 +2493,7 @@
         <v>9570</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>